<commit_message>
ENH: Add PnlType field to AocType
</commit_message>
<xml_diff>
--- a/lifelib/libraries/ifrs17a/Files/ifrs17-template/Dimensions.xlsx
+++ b/lifelib/libraries/ifrs17a/Files/ifrs17-template/Dimensions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fumito\OneDrive\pyproj\IFRS17CalculationEnginePython\ifrs17_template\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e058ec69bd94c7d/pyproj/lifelib/lifelib/libraries/ifrs17a/Files/ifrs17-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B358B30E-E1BD-4739-B05C-FBF4E1A5BE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{B358B30E-E1BD-4739-B05C-FBF4E1A5BE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7C0D06B-EAE9-4243-8309-353883BB6A22}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="768" activeTab="9" xr2:uid="{306A9329-EBFE-4F70-A441-0C01444228B5}"/>
+    <workbookView xWindow="2109" yWindow="566" windowWidth="29082" windowHeight="16954" tabRatio="768" firstSheet="3" activeTab="3" xr2:uid="{306A9329-EBFE-4F70-A441-0C01444228B5}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingNode" sheetId="21" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="386">
   <si>
     <t>SystemName</t>
   </si>
@@ -1205,6 +1205,26 @@
   </si>
   <si>
     <t>Opening, Actual</t>
+  </si>
+  <si>
+    <t>PnlType</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FX</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1560,7 +1580,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1574,9 +1594,9 @@
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1590,7 +1610,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>356</v>
       </c>
@@ -1601,7 +1621,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>358</v>
       </c>
@@ -1615,7 +1635,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1629,7 +1649,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>361</v>
       </c>
@@ -1643,7 +1663,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>363</v>
       </c>
@@ -1657,7 +1677,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>365</v>
       </c>
@@ -1671,7 +1691,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>367</v>
       </c>
@@ -1685,7 +1705,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>369</v>
       </c>
@@ -1709,13 +1729,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66956434-E951-451B-9993-178F88BD0387}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1746,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -1734,7 +1754,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>178</v>
       </c>
@@ -1756,9 +1776,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1772,7 +1792,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -1783,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -1797,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>184</v>
       </c>
@@ -1811,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -1825,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -1839,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>190</v>
       </c>
@@ -1853,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>192</v>
       </c>
@@ -1867,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>194</v>
       </c>
@@ -1881,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>196</v>
       </c>
@@ -1895,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
         <v>198</v>
       </c>
@@ -1909,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
         <v>200</v>
       </c>
@@ -1923,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
         <v>202</v>
       </c>
@@ -1937,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
         <v>204</v>
       </c>
@@ -1951,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
         <v>206</v>
       </c>
@@ -1965,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A16" t="s">
         <v>208</v>
       </c>
@@ -1993,9 +2013,9 @@
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2017,7 +2037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -2028,7 +2048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2053,9 +2073,9 @@
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2063,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>213</v>
       </c>
@@ -2085,9 +2105,9 @@
       <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2095,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -2117,9 +2137,9 @@
       <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2133,7 +2153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>216</v>
       </c>
@@ -2158,9 +2178,9 @@
       <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>218</v>
       </c>
@@ -2185,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>220</v>
       </c>
@@ -2199,7 +2219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>221</v>
       </c>
@@ -2213,7 +2233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>223</v>
       </c>
@@ -2227,7 +2247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>225</v>
       </c>
@@ -2241,7 +2261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>227</v>
       </c>
@@ -2255,7 +2275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>228</v>
       </c>
@@ -2269,7 +2289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>230</v>
       </c>
@@ -2283,7 +2303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>232</v>
       </c>
@@ -2297,7 +2317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
         <v>234</v>
       </c>
@@ -2311,7 +2331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
         <v>236</v>
       </c>
@@ -2325,7 +2345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
         <v>238</v>
       </c>
@@ -2339,7 +2359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
         <v>240</v>
       </c>
@@ -2353,7 +2373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
         <v>242</v>
       </c>
@@ -2367,7 +2387,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A16" t="s">
         <v>243</v>
       </c>
@@ -2381,7 +2401,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A17" t="s">
         <v>245</v>
       </c>
@@ -2395,7 +2415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A18" t="s">
         <v>247</v>
       </c>
@@ -2409,7 +2429,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -2423,7 +2443,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -2437,7 +2457,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A21" t="s">
         <v>252</v>
       </c>
@@ -2451,7 +2471,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A22" t="s">
         <v>254</v>
       </c>
@@ -2465,7 +2485,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A23" t="s">
         <v>256</v>
       </c>
@@ -2479,7 +2499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A24" t="s">
         <v>258</v>
       </c>
@@ -2493,7 +2513,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A25" t="s">
         <v>260</v>
       </c>
@@ -2507,7 +2527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A26" t="s">
         <v>262</v>
       </c>
@@ -2521,7 +2541,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A27" t="s">
         <v>264</v>
       </c>
@@ -2535,7 +2555,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A28" t="s">
         <v>266</v>
       </c>
@@ -2549,7 +2569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A29" t="s">
         <v>268</v>
       </c>
@@ -2563,7 +2583,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A30" t="s">
         <v>270</v>
       </c>
@@ -2577,7 +2597,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A31" t="s">
         <v>271</v>
       </c>
@@ -2591,7 +2611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A32" t="s">
         <v>272</v>
       </c>
@@ -2619,9 +2639,9 @@
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2629,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -2637,7 +2657,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>275</v>
       </c>
@@ -2645,7 +2665,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>277</v>
       </c>
@@ -2667,9 +2687,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2683,7 +2703,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>213</v>
       </c>
@@ -2708,9 +2728,9 @@
       <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2718,7 +2738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -2726,7 +2746,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>281</v>
       </c>
@@ -2734,7 +2754,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>283</v>
       </c>
@@ -2742,7 +2762,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>285</v>
       </c>
@@ -2750,7 +2770,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>287</v>
       </c>
@@ -2758,7 +2778,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>289</v>
       </c>
@@ -2766,7 +2786,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>291</v>
       </c>
@@ -2774,7 +2794,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>293</v>
       </c>
@@ -2782,7 +2802,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>295</v>
       </c>
@@ -2790,7 +2810,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
         <v>297</v>
       </c>
@@ -2798,7 +2818,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
         <v>299</v>
       </c>
@@ -2806,7 +2826,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
         <v>301</v>
       </c>
@@ -2814,7 +2834,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
         <v>303</v>
       </c>
@@ -2822,7 +2842,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
         <v>305</v>
       </c>
@@ -2830,7 +2850,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A16" t="s">
         <v>307</v>
       </c>
@@ -2838,7 +2858,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A17" t="s">
         <v>309</v>
       </c>
@@ -2860,9 +2880,9 @@
       <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2891,7 +2911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2917,7 +2937,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2931,7 +2951,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2960,7 +2980,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2983,7 +3003,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -3000,7 +3020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -3017,7 +3037,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -3034,7 +3054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -3051,7 +3071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -3065,7 +3085,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -3082,7 +3102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -3099,7 +3119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -3113,7 +3133,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -3127,7 +3147,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -3144,7 +3164,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -3175,9 +3195,9 @@
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3185,7 +3205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>311</v>
       </c>
@@ -3207,9 +3227,9 @@
       <selection activeCell="K23" sqref="K22:K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3223,7 +3243,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>315</v>
       </c>
@@ -3237,7 +3257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>317</v>
       </c>
@@ -3251,7 +3271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>319</v>
       </c>
@@ -3265,7 +3285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>321</v>
       </c>
@@ -3279,7 +3299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>323</v>
       </c>
@@ -3293,7 +3313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>325</v>
       </c>
@@ -3307,7 +3327,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>327</v>
       </c>
@@ -3321,7 +3341,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>329</v>
       </c>
@@ -3335,7 +3355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>331</v>
       </c>
@@ -3349,7 +3369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
         <v>333</v>
       </c>
@@ -3363,7 +3383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
         <v>335</v>
       </c>
@@ -3377,7 +3397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
         <v>337</v>
       </c>
@@ -3391,7 +3411,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
         <v>339</v>
       </c>
@@ -3405,7 +3425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
         <v>341</v>
       </c>
@@ -3419,7 +3439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A16" t="s">
         <v>343</v>
       </c>
@@ -3433,7 +3453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A17" t="s">
         <v>345</v>
       </c>
@@ -3447,7 +3467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A18" t="s">
         <v>347</v>
       </c>
@@ -3461,7 +3481,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A19" t="s">
         <v>349</v>
       </c>
@@ -3475,7 +3495,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A20" t="s">
         <v>351</v>
       </c>
@@ -3489,7 +3509,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A21" t="s">
         <v>353</v>
       </c>
@@ -3517,9 +3537,9 @@
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3536,7 +3556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -3550,7 +3570,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -3575,15 +3595,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4750F88B-153B-4CC9-94C0-4D86A6CC0B01}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
+  <cols>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3596,8 +3619,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -3607,8 +3633,11 @@
       <c r="D2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -3618,8 +3647,11 @@
       <c r="D3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -3629,8 +3661,11 @@
       <c r="D4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -3643,8 +3678,11 @@
       <c r="D5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -3654,8 +3692,11 @@
       <c r="D6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -3665,8 +3706,11 @@
       <c r="D7">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -3676,8 +3720,11 @@
       <c r="D8">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -3687,8 +3734,11 @@
       <c r="D9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -3701,8 +3751,11 @@
       <c r="D10">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -3715,8 +3768,11 @@
       <c r="D11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -3726,8 +3782,11 @@
       <c r="D12">
         <v>110</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -3737,8 +3796,11 @@
       <c r="D13">
         <v>120</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -3748,8 +3810,11 @@
       <c r="D14">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -3759,8 +3824,11 @@
       <c r="D15">
         <v>140</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -3770,8 +3838,11 @@
       <c r="D16">
         <v>150</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -3781,8 +3852,11 @@
       <c r="D17">
         <v>160</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -3807,12 +3881,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="4" max="4" width="16.9140625" customWidth="1"/>
+    <col min="4" max="4" width="16.92578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -3850,7 +3924,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -3888,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -3926,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -3964,7 +4038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -4002,7 +4076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -4040,7 +4114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -4078,7 +4152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -4116,7 +4190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -4154,7 +4228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -4192,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -4230,7 +4304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -4268,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -4306,7 +4380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -4344,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -4382,7 +4456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -4420,7 +4494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -4458,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -4496,7 +4570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -4534,7 +4608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -4572,7 +4646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -4610,7 +4684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -4662,9 +4736,9 @@
       <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4672,7 +4746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -4680,7 +4754,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -4688,7 +4762,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -4696,7 +4770,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -4704,7 +4778,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -4712,7 +4786,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -4720,7 +4794,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -4728,7 +4802,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -4736,7 +4810,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -4744,7 +4818,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -4752,7 +4826,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -4760,7 +4834,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -4768,7 +4842,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -4776,7 +4850,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -4784,7 +4858,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -4792,7 +4866,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -4800,7 +4874,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -4808,7 +4882,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -4816,7 +4890,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -4824,7 +4898,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -4832,7 +4906,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -4840,7 +4914,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -4862,9 +4936,9 @@
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4872,7 +4946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -4880,7 +4954,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -4888,7 +4962,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -4896,7 +4970,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>134</v>
       </c>
@@ -4904,7 +4978,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -4912,7 +4986,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -4920,7 +4994,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -4928,7 +5002,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -4936,7 +5010,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -4958,9 +5032,9 @@
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4968,7 +5042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -4976,7 +5050,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -4984,7 +5058,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -5006,12 +5080,12 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="5" max="5" width="19.2109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5046,7 +5120,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -5066,7 +5140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -5086,7 +5160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
         <v>157</v>
       </c>
@@ -5106,7 +5180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -5126,7 +5200,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -5146,7 +5220,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -5166,7 +5240,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -5186,7 +5260,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -5221,7 +5295,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -5256,7 +5330,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -5276,7 +5350,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -5296,7 +5370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
         <v>172</v>
       </c>
@@ -5316,7 +5390,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
         <v>174</v>
       </c>
@@ -5336,7 +5410,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
         <v>175</v>
       </c>

</xml_diff>